<commit_message>
edit: Edit water bill model and query water bill
</commit_message>
<xml_diff>
--- a/app/resources/templates/water_bill_template.xlsx
+++ b/app/resources/templates/water_bill_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yongp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yongp\OneDrive\Documents\GitHub\fastapi_demo\app\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3916B05-56FC-4C1C-8249-96C1DC6F34FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA69D19-F46A-46AF-830C-64B156D68A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7116" yWindow="3480" windowWidth="17280" windowHeight="8964" xr2:uid="{43D2934B-19C8-4FA4-85A3-A5B17E6B9BD6}"/>
+    <workbookView xWindow="3684" yWindow="2772" windowWidth="17280" windowHeight="8964" xr2:uid="{43D2934B-19C8-4FA4-85A3-A5B17E6B9BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Tên người dùng</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Ngày tạo đơn</t>
+  </si>
+  <si>
+    <t>Người tạo</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7368F2-BD19-4D59-8418-206DA4899292}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,7 +491,7 @@
     <col min="9" max="9" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -515,6 +518,9 @@
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>